<commit_message>
Fix calculations for AWS
</commit_message>
<xml_diff>
--- a/hw_1/Pricing_calculation.xlsx
+++ b/hw_1/Pricing_calculation.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrey/Documents/Coding/GL-DevOps-BaseCamp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrey/Documents/Coding/GL-DevOps-BaseCamp/hw_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C0E932A-68A0-0746-BB46-4DB23C05E4F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAD5B9B0-DA78-5E4C-A6A2-1ED4B7254099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{EAC4C1C5-9678-4846-8A35-1131869B1DC6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -101,9 +101,6 @@
     <t>EC2 instance (Reserved - 1 year - eu-central-1) - t3.xlarge (4vCPU - 16GiB)</t>
   </si>
   <si>
-    <t>1 month</t>
-  </si>
-  <si>
     <t>1 year</t>
   </si>
   <si>
@@ -125,7 +122,10 @@
     <t>Amazon S3 (1TB - 10 million requests per month)</t>
   </si>
   <si>
-    <t>Amazon ELB (price depends on network traffic) x12</t>
+    <t>12 month</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amazon ELB (price depends on network traffic) </t>
   </si>
 </sst>
 </file>
@@ -133,7 +133,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="_-* #,##0.00\ [$USD]_-;\-* #,##0.00\ [$USD]_-;_-* &quot;-&quot;??\ [$USD]_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$USD]_-;\-* #,##0.00\ [$USD]_-;_-* &quot;-&quot;??\ [$USD]_-;_-@_-"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -495,169 +495,166 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -977,7 +974,7 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -988,530 +985,588 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="11"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="49"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="41"/>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="42"/>
+      <c r="A2" s="50"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="51"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="13"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="53"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="39"/>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="40"/>
+      <c r="A4" s="54"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="55"/>
     </row>
     <row r="5" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="7" t="s">
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="1" t="s">
+      <c r="H5" s="47"/>
+      <c r="I5" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="J5" s="14"/>
+      <c r="J5" s="56"/>
     </row>
     <row r="6" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="8">
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="4">
         <v>2</v>
       </c>
-      <c r="H6" s="9"/>
-      <c r="I6" s="24">
+      <c r="H6" s="5"/>
+      <c r="I6" s="1">
         <v>2178</v>
       </c>
-      <c r="J6" s="25"/>
+      <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="8">
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="4">
         <v>1</v>
       </c>
-      <c r="H7" s="9"/>
-      <c r="I7" s="24">
+      <c r="H7" s="5"/>
+      <c r="I7" s="1">
         <v>1089</v>
       </c>
-      <c r="J7" s="25"/>
+      <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="8">
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="4">
         <v>2</v>
       </c>
-      <c r="H8" s="9"/>
-      <c r="I8" s="24">
+      <c r="H8" s="5"/>
+      <c r="I8" s="1">
         <v>427</v>
       </c>
-      <c r="J8" s="25"/>
+      <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="8">
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="4">
         <v>3</v>
       </c>
-      <c r="H9" s="9"/>
-      <c r="I9" s="24">
+      <c r="H9" s="5"/>
+      <c r="I9" s="1">
         <v>1000</v>
       </c>
-      <c r="J9" s="25"/>
+      <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="8">
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="4">
         <v>2</v>
       </c>
-      <c r="H10" s="9"/>
-      <c r="I10" s="24">
+      <c r="H10" s="5"/>
+      <c r="I10" s="1">
         <v>800</v>
       </c>
-      <c r="J10" s="25"/>
+      <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="8">
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="4">
         <v>2</v>
       </c>
-      <c r="H11" s="9"/>
-      <c r="I11" s="24">
+      <c r="H11" s="5"/>
+      <c r="I11" s="1">
         <v>118</v>
       </c>
-      <c r="J11" s="25"/>
+      <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="8">
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="4">
         <v>1</v>
       </c>
-      <c r="H12" s="9"/>
-      <c r="I12" s="24">
+      <c r="H12" s="5"/>
+      <c r="I12" s="1">
         <v>52</v>
       </c>
-      <c r="J12" s="25"/>
+      <c r="J12" s="2"/>
     </row>
     <row r="13" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="8">
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="4">
         <v>2</v>
       </c>
-      <c r="H13" s="9"/>
-      <c r="I13" s="24">
+      <c r="H13" s="5"/>
+      <c r="I13" s="1">
         <v>460</v>
       </c>
-      <c r="J13" s="25"/>
+      <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="8">
+      <c r="A14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="4">
         <v>1</v>
       </c>
-      <c r="H14" s="9"/>
-      <c r="I14" s="26">
+      <c r="H14" s="5"/>
+      <c r="I14" s="6">
         <v>448</v>
       </c>
-      <c r="J14" s="25"/>
+      <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="8" t="s">
+      <c r="A15" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H15" s="9"/>
-      <c r="I15" s="24">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="5"/>
+      <c r="I15" s="1">
         <v>12</v>
       </c>
-      <c r="J15" s="25"/>
+      <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="8">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="4">
         <v>2</v>
       </c>
-      <c r="H16" s="9"/>
-      <c r="I16" s="26">
+      <c r="H16" s="5"/>
+      <c r="I16" s="6">
         <v>200</v>
       </c>
-      <c r="J16" s="25"/>
+      <c r="J16" s="2"/>
     </row>
     <row r="17" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="1">
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="46">
         <v>1</v>
       </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="27">
+      <c r="H17" s="47"/>
+      <c r="I17" s="42">
         <v>100</v>
       </c>
-      <c r="J17" s="28"/>
+      <c r="J17" s="43"/>
     </row>
     <row r="18" spans="1:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="32">
+      <c r="B18" s="39"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="44">
         <f>SUM(I6:J17)</f>
         <v>6884</v>
       </c>
-      <c r="J18" s="33"/>
+      <c r="J18" s="45"/>
     </row>
     <row r="19" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A19" s="49" t="s">
+      <c r="A19" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="49"/>
-      <c r="C19" s="49"/>
-      <c r="D19" s="49"/>
-      <c r="E19" s="49"/>
-      <c r="F19" s="50"/>
-      <c r="G19" s="22" t="s">
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="H19" s="23"/>
-      <c r="I19" s="29">
+      <c r="H19" s="20"/>
+      <c r="I19" s="31">
         <v>810</v>
       </c>
-      <c r="J19" s="30"/>
+      <c r="J19" s="32"/>
     </row>
     <row r="20" spans="1:10" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="34" t="s">
+      <c r="A20" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="35"/>
-      <c r="I20" s="31">
+      <c r="B20" s="33"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="35">
         <v>810</v>
       </c>
       <c r="J20" s="36"/>
     </row>
     <row r="21" spans="1:10" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="37" t="s">
+      <c r="A21" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="37"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="37"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="37"/>
-      <c r="G21" s="37"/>
-      <c r="H21" s="38"/>
-      <c r="I21" s="47">
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="9">
         <f>SUM(I18,I20)</f>
         <v>7694</v>
       </c>
-      <c r="J21" s="48"/>
+      <c r="J21" s="10"/>
     </row>
     <row r="22" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="43" t="s">
+      <c r="A22" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="43"/>
-      <c r="C22" s="43"/>
-      <c r="D22" s="43"/>
-      <c r="E22" s="43"/>
-      <c r="F22" s="43"/>
-      <c r="G22" s="43"/>
-      <c r="H22" s="43"/>
-      <c r="I22" s="43"/>
-      <c r="J22" s="44"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="16"/>
     </row>
     <row r="23" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="45"/>
-      <c r="B23" s="45"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="45"/>
-      <c r="G23" s="45"/>
-      <c r="H23" s="45"/>
-      <c r="I23" s="45"/>
-      <c r="J23" s="46"/>
+      <c r="A23" s="17"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="18"/>
     </row>
     <row r="24" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="20"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="22" t="s">
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="H24" s="23"/>
-      <c r="I24" s="22" t="s">
+      <c r="H24" s="20"/>
+      <c r="I24" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="J24" s="57"/>
+      <c r="J24" s="22"/>
     </row>
     <row r="25" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A25" s="55" t="s">
+      <c r="A25" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="55"/>
-      <c r="C25" s="55"/>
-      <c r="D25" s="55"/>
-      <c r="E25" s="55"/>
-      <c r="F25" s="56"/>
-      <c r="G25" s="53">
+      <c r="B25" s="23"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="25">
         <v>2</v>
       </c>
-      <c r="H25" s="54"/>
-      <c r="I25" s="51">
+      <c r="H25" s="26"/>
+      <c r="I25" s="27">
         <v>1970</v>
       </c>
-      <c r="J25" s="52"/>
+      <c r="J25" s="28"/>
     </row>
     <row r="26" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="H26" s="9"/>
-      <c r="I26" s="26">
-        <v>200</v>
-      </c>
-      <c r="J26" s="25"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H26" s="5"/>
+      <c r="I26" s="6">
+        <v>1200</v>
+      </c>
+      <c r="J26" s="2"/>
     </row>
     <row r="27" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="4">
+        <v>1</v>
+      </c>
+      <c r="H27" s="5"/>
+      <c r="I27" s="6">
+        <v>0</v>
+      </c>
+      <c r="J27" s="2"/>
+    </row>
+    <row r="28" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="A28" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="8">
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="4">
         <v>1</v>
       </c>
-      <c r="H27" s="9"/>
-      <c r="I27" s="26">
+      <c r="H28" s="5"/>
+      <c r="I28" s="6">
+        <v>12</v>
+      </c>
+      <c r="J28" s="2"/>
+    </row>
+    <row r="29" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="A29" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="4">
+        <v>1</v>
+      </c>
+      <c r="H29" s="5"/>
+      <c r="I29" s="6">
         <v>0</v>
       </c>
-      <c r="J27" s="25"/>
-    </row>
-    <row r="28" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+      <c r="J29" s="2"/>
+    </row>
+    <row r="30" spans="1:10" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="8">
-        <v>1</v>
-      </c>
-      <c r="H28" s="9"/>
-      <c r="I28" s="26">
-        <v>12</v>
-      </c>
-      <c r="J28" s="25"/>
-    </row>
-    <row r="29" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="8">
-        <v>1</v>
-      </c>
-      <c r="H29" s="9"/>
-      <c r="I29" s="26">
-        <v>0</v>
-      </c>
-      <c r="J29" s="25"/>
-    </row>
-    <row r="30" spans="1:10" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="58" t="s">
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="58"/>
-      <c r="C30" s="58"/>
-      <c r="D30" s="58"/>
-      <c r="E30" s="58"/>
-      <c r="F30" s="58"/>
-      <c r="G30" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="H30" s="9"/>
-      <c r="I30" s="26">
-        <v>29</v>
-      </c>
-      <c r="J30" s="25"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="6">
+        <v>450</v>
+      </c>
+      <c r="J30" s="2"/>
     </row>
     <row r="31" spans="1:10" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="37" t="s">
+      <c r="A31" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B31" s="37"/>
-      <c r="C31" s="37"/>
-      <c r="D31" s="37"/>
-      <c r="E31" s="37"/>
-      <c r="F31" s="37"/>
-      <c r="G31" s="37"/>
-      <c r="H31" s="38"/>
-      <c r="I31" s="47">
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="9">
         <f>SUM(I25:J30)</f>
-        <v>2211</v>
-      </c>
-      <c r="J31" s="48"/>
+        <v>3632</v>
+      </c>
+      <c r="J31" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="74">
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="A1:J2"/>
+    <mergeCell ref="A3:J4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="A14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="A17:F17"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="A20:H20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="A22:J23"/>
+    <mergeCell ref="A24:F24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="A25:F25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="I25:J25"/>
     <mergeCell ref="I13:J13"/>
     <mergeCell ref="A30:F30"/>
     <mergeCell ref="G30:H30"/>
@@ -1528,64 +1583,6 @@
     <mergeCell ref="G26:H26"/>
     <mergeCell ref="I26:J26"/>
     <mergeCell ref="A27:F27"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="A22:J23"/>
-    <mergeCell ref="A24:F24"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="A25:F25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="A20:H20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="A17:F17"/>
-    <mergeCell ref="A18:H18"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="A16:F16"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="A12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="A15:F15"/>
-    <mergeCell ref="A14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="A13:F13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="A1:J2"/>
-    <mergeCell ref="A3:J4"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A6:F6" r:id="rId1" location="techspecs_section" display="DELL PowerEdge R250 Rack Server (servers)" xr:uid="{5266694F-7C10-2341-9FDE-1807A4A0250A}"/>

</xml_diff>